<commit_message>
Draw chart with PhpSpreadsheet
</commit_message>
<xml_diff>
--- a/posts/php - excel/phpspreadsheet/chart_output.xlsx
+++ b/posts/php - excel/phpspreadsheet/chart_output.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView activeTab="1" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
@@ -27,7 +27,7 @@
     <t>Anna</t>
   </si>
   <si>
-    <t>Bob</t>
+    <t>Bình</t>
   </si>
   <si>
     <t>Clark</t>
@@ -89,6 +89,168 @@
   <dxfs count="0"/>
   <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr b="0" i="0" u="none" strike="noStrike">
+                <a:latin typeface="Calibri"/>
+              </a:rPr>
+              <a:t/>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout/>
+      </c:layout>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF9900"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet2!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Anna</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Bình</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Clark</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$2:$B$4</c:f>
+              <c:numCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins footer="0.3" header="0.3" r="0.7" l="0.7" t="0.75" b="0.75"/>
+    <c:pageSetup orientation="portrait"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr name="Chart 1" id="1025"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -383,7 +545,7 @@
   </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
@@ -439,7 +601,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>90</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:2">

</xml_diff>